<commit_message>
Added 25-27 April Experimental Data
- BCM files
- Updated foil speadsheets
</commit_message>
<xml_diff>
--- a/Experiments/Activation/33MeVTa_25Apr/BeamOnlyData/BeamFoilDimensions.xlsx
+++ b/Experiments/Activation/33MeVTa_25Apr/BeamOnlyData/BeamFoilDimensions.xlsx
@@ -381,7 +381,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,6 +459,10 @@
         <f>F2/((B2/20)^2*3.1415*D2/10)</f>
         <v>6.5098944770896319</v>
       </c>
+      <c r="I2">
+        <f>SQRT((C2/B2)^2+(E2/D2)^2+(G2/F2)^2)*H2</f>
+        <v>1.4193727148515141E-2</v>
+      </c>
       <c r="J2">
         <v>0.98850000000000005</v>
       </c>
@@ -489,6 +493,10 @@
         <f>F3/((B3/20)^2*3.1415*D3/10)</f>
         <v>7.1036287670575256</v>
       </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I6" si="0">SQRT((C3/B3)^2+(E3/D3)^2+(G3/F3)^2)*H3</f>
+        <v>3.7573945915260518E-2</v>
+      </c>
       <c r="J3">
         <v>0.99999000000000005</v>
       </c>
@@ -519,6 +527,10 @@
         <f>F4/((B4/20)^2*3.1415*D4/10)</f>
         <v>8.7997854746995028</v>
       </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>3.184399701236567E-2</v>
+      </c>
       <c r="J4">
         <v>0.98980000000000001</v>
       </c>
@@ -549,6 +561,10 @@
         <f>F5/((B5/20)^2*3.1415*D5/10)</f>
         <v>18.343044133302069</v>
       </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0.58670055427926948</v>
+      </c>
       <c r="J5">
         <v>0.999</v>
       </c>
@@ -581,6 +597,10 @@
       <c r="H6">
         <f>F6/((B6/20)^2*3.1415*D6/10)</f>
         <v>2.667722912655925</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>9.5862100566469211E-3</v>
       </c>
       <c r="J6">
         <v>0.99999000000000005</v>

</xml_diff>

<commit_message>
Updated beam only MCNP results.
   - Modified experimental geometry
   - Reran simulation
   - Added analysis notebook just for initial activities
</commit_message>
<xml_diff>
--- a/Experiments/Activation/33MeVTa_25Apr/BeamOnlyData/BeamFoilDimensions.xlsx
+++ b/Experiments/Activation/33MeVTa_25Apr/BeamOnlyData/BeamFoilDimensions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Thickness (mm)</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Foil</t>
   </si>
   <si>
-    <t>Circumference (mm)</t>
-  </si>
-  <si>
     <t>Uncertainty</t>
   </si>
   <si>
@@ -61,6 +58,21 @@
   </si>
   <si>
     <t>impurity questionable</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Density Uncertainty</t>
+  </si>
+  <si>
+    <t>Volume Uncertainty</t>
+  </si>
+  <si>
+    <t>Volume [cm^3]</t>
+  </si>
+  <si>
+    <t>Diameter (mm)</t>
   </si>
 </sst>
 </file>
@@ -96,8 +108,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,64 +393,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+    </row>
+    <row r="2" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>8</v>
       </c>
       <c r="B2">
         <v>49.9</v>
@@ -456,20 +479,28 @@
         <v>2E-3</v>
       </c>
       <c r="H2">
+        <f>PI()*B2^2/4*D2/1000</f>
+        <v>2.0260526549515663</v>
+      </c>
+      <c r="I2">
+        <f>SQRT((C2/B2)^2+(E2/D2)^2)*H2</f>
+        <v>4.4067691960275011E-3</v>
+      </c>
+      <c r="J2">
         <f>F2/((B2/20)^2*3.1415*D2/10)</f>
         <v>6.5098944770896319</v>
       </c>
-      <c r="I2">
-        <f>SQRT((C2/B2)^2+(E2/D2)^2+(G2/F2)^2)*H2</f>
+      <c r="K2">
+        <f>SQRT((C2/B2)^2+(E2/D2)^2+(G2/F2)^2)*J2</f>
         <v>1.4193727148515141E-2</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>0.98850000000000005</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>50.15</v>
@@ -490,20 +521,28 @@
         <v>2E-3</v>
       </c>
       <c r="H3">
+        <f t="shared" ref="H3:H6" si="0">PI()*B3^2/4*D3/1000</f>
+        <v>2.0167752275037274</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I6" si="1">SQRT((C3/B3)^2+(E3/D3)^2)*H3</f>
+        <v>1.0663818005793763E-2</v>
+      </c>
+      <c r="J3">
         <f>F3/((B3/20)^2*3.1415*D3/10)</f>
         <v>7.1036287670575256</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I6" si="0">SQRT((C3/B3)^2+(E3/D3)^2+(G3/F3)^2)*H3</f>
+      <c r="K3">
+        <f t="shared" ref="K3:K6" si="2">SQRT((C3/B3)^2+(E3/D3)^2+(G3/F3)^2)*J3</f>
         <v>3.7573945915260518E-2</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>0.99999000000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>49.5</v>
@@ -524,20 +563,28 @@
         <v>2E-3</v>
       </c>
       <c r="H4">
+        <f t="shared" si="0"/>
+        <v>1.9244218498645975</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>6.9602420195695978E-3</v>
+      </c>
+      <c r="J4">
         <f>F4/((B4/20)^2*3.1415*D4/10)</f>
         <v>8.7997854746995028</v>
       </c>
-      <c r="I4">
-        <f t="shared" si="0"/>
+      <c r="K4">
+        <f t="shared" si="2"/>
         <v>3.184399701236567E-2</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>0.98980000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>49.35</v>
@@ -558,23 +605,31 @@
         <v>2E-3</v>
       </c>
       <c r="H5">
+        <f t="shared" si="0"/>
+        <v>0.17980097770810127</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>5.7498837395438809E-3</v>
+      </c>
+      <c r="J5">
         <f>F5/((B5/20)^2*3.1415*D5/10)</f>
         <v>18.343044133302069</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
+      <c r="K5">
+        <f t="shared" si="2"/>
         <v>0.58670055427926948</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>0.999</v>
       </c>
-      <c r="K5" t="s">
-        <v>13</v>
+      <c r="M5" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>50</v>
@@ -595,18 +650,32 @@
         <v>2E-3</v>
       </c>
       <c r="H6">
+        <f t="shared" si="0"/>
+        <v>1.9890208488040375</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>7.1079282298352102E-3</v>
+      </c>
+      <c r="J6">
         <f>F6/((B6/20)^2*3.1415*D6/10)</f>
         <v>2.667722912655925</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
+      <c r="K6">
+        <f t="shared" si="2"/>
         <v>9.5862100566469211E-3</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>0.99999000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>